<commit_message>
改名字 kick off message
</commit_message>
<xml_diff>
--- a/game_sample/excel/game_sample.xlsx
+++ b/game_sample/excel/game_sample.xlsx
@@ -33,42 +33,42 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={D0BBDEBC-BE72-4AD2-8219-85103BCEC826}</author>
-    <author>tc={747DB93C-7AB1-47E5-9B16-39AF33E4A745}</author>
-    <author>tc={4F7A6503-4435-493C-80CA-7CD4776E9D86}</author>
-    <author>tc={9EC03FE5-AE0D-4C90-B1F6-AEC8B446BA1B}</author>
-    <author>tc={E48C8BDD-69FC-441A-878D-29B5FC86193F}</author>
-    <author>tc={46F01611-4B57-49A7-8822-06A5CEC7A7E6}</author>
+    <author>tc={4888C72F-844C-4E42-A1E0-7E513E46E074}</author>
+    <author>tc={DEF321D1-9D6A-4F79-8C91-5D51D6D63DC6}</author>
+    <author>tc={9F468E66-502E-4E4E-B896-B7E9B9DE272C}</author>
+    <author>tc={8BB45A2E-51CB-455A-A5DB-147EB3B9AE92}</author>
+    <author>tc={D3C47417-4673-4518-AB61-84FCB80655CD}</author>
+    <author>tc={EB3B585F-507F-4522-85A7-B6D82D7557C9}</author>
   </authors>
   <commentList>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{D0BBDEBC-BE72-4AD2-8219-85103BCEC826}">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{4888C72F-844C-4E42-A1E0-7E513E46E074}">
+      <text>
+        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @宾晓华 step4: 这个是角色启动提示词，可以看到鼠王和小灰鼠的关系做再次强调。</t>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="1" shapeId="0" xr:uid="{DEF321D1-9D6A-4F79-8C91-5D51D6D63DC6}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @宾晓华 step3: 这个是角色启动的提示词设置，可以看到小老鼠和鼠王的关系。</t>
       </text>
     </comment>
-    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{747DB93C-7AB1-47E5-9B16-39AF33E4A745}">
-      <text>
-        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 这个部分可以看到，鼠王和小老鼠的设计。</t>
-      </text>
-    </comment>
-    <comment ref="H9" authorId="2" shapeId="0" xr:uid="{4F7A6503-4435-493C-80CA-7CD4776E9D86}">
-      <text>
-        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @宾晓华 step4: 这个是角色启动提示词，可以看到鼠王和小灰鼠的关系做再次强调。</t>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="3" shapeId="0" xr:uid="{9EC03FE5-AE0D-4C90-B1F6-AEC8B446BA1B}">
+    <comment ref="A4" authorId="2" shapeId="0" xr:uid="{9F468E66-502E-4E4E-B896-B7E9B9DE272C}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @侯清辰 先忽略。我改了gen_game。也测试了，不会炸了</t>
       </text>
     </comment>
-    <comment ref="K1" authorId="4" shapeId="0" xr:uid="{E48C8BDD-69FC-441A-878D-29B5FC86193F}">
+    <comment ref="J1" authorId="3" shapeId="0" xr:uid="{8BB45A2E-51CB-455A-A5DB-147EB3B9AE92}">
+      <text>
+        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 写在这里是因为后续希望做：外貌会随着装备而改变。就是受到装备的影响。 Reply: 空着，运行中会通过LLM自主运行成功</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="4" shapeId="0" xr:uid="{D3C47417-4673-4518-AB61-84FCB80655CD}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @侯清辰 挪到这里了～程序我这边来改</t>
       </text>
     </comment>
-    <comment ref="J1" authorId="5" shapeId="0" xr:uid="{46F01611-4B57-49A7-8822-06A5CEC7A7E6}">
+    <comment ref="C2" authorId="5" shapeId="0" xr:uid="{EB3B585F-507F-4522-85A7-B6D82D7557C9}">
       <text>
-        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 写在这里是因为后续希望做：外貌会随着装备而改变。就是受到装备的影响。 Reply: 空着，运行中会通过LLM自主运行成功</t>
+        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 这个部分可以看到，鼠王和小老鼠的设计。</t>
       </text>
     </comment>
   </commentList>
@@ -78,10 +78,10 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={3E209442-526B-44C8-B09D-EA0B4907C6D6}</author>
+    <author>tc={408F8C31-42B8-4F84-87D2-92DC1AF46779}</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{3E209442-526B-44C8-B09D-EA0B4907C6D6}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{408F8C31-42B8-4F84-87D2-92DC1AF46779}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @宾晓华 这里</t>
       </text>
@@ -93,22 +93,22 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={E4F17891-16D4-4721-869E-FF593C4C51D8}</author>
-    <author>tc={B5F08C40-83C5-4264-8A42-E9EDAA04429E}</author>
-    <author>tc={14C968F9-8D8D-4C80-8F9D-7AC2DE93639E}</author>
+    <author>tc={9A2C7972-00D8-4052-BDCB-DB2E267D6D66}</author>
+    <author>tc={96025EC3-3895-47B1-B2CC-F5CE7AF733E9}</author>
+    <author>tc={24D52379-8453-4DE7-83F4-258872B8BD1A}</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{E4F17891-16D4-4721-869E-FF593C4C51D8}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{9A2C7972-00D8-4052-BDCB-DB2E267D6D66}">
+      <text>
+        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @宾晓华 这里</t>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="1" shapeId="0" xr:uid="{96025EC3-3895-47B1-B2CC-F5CE7AF733E9}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @宾晓华  step1: system 级提示词。具体看内容。里面“子嗣”在暗示社会关系。但是这里是故意的：暗示鼠王有很多孩子，小灰鼠帕奇只是其中之一。</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{B5F08C40-83C5-4264-8A42-E9EDAA04429E}">
-      <text>
-        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @宾晓华 这里</t>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="2" shapeId="0" xr:uid="{14C968F9-8D8D-4C80-8F9D-7AC2DE93639E}">
+    <comment ref="C6" authorId="2" shapeId="0" xr:uid="{24D52379-8453-4DE7-83F4-258872B8BD1A}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @宾晓华 step2：小灰鼠帕奇的，系统级提示词，可以看到鼠王是父亲。</t>
       </text>
@@ -120,22 +120,22 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={13FB0462-67E8-40DB-8A1B-3DD1C7B7BB1B}</author>
-    <author>tc={57F1A3C5-98B0-4856-B23C-77BDF2B931AB}</author>
+    <author>tc={5C7CD0B5-8E8B-4022-BB1E-0E2A44212101}</author>
+    <author>tc={836141CE-64F2-47A4-B0CC-32CBA2F438BF}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{13FB0462-67E8-40DB-8A1B-3DD1C7B7BB1B}">
-      <text>
-        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 世界独一无二，基本是影响游戏流程的东西。如果标记Yes，就可以被战斗杀死抢夺</t>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{57F1A3C5-98B0-4856-B23C-77BDF2B931AB}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{5C7CD0B5-8E8B-4022-BB1E-0E2A44212101}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: RoleComponent, 角色的一部分，不可分割
 Weapon，武器，可能用于战斗
 Clothes，全身套装，影响外观
 NonConsumableItem，不可消耗的东西，例如钥匙。后续会有可消耗的东西
 Event，发生的事件 Reply: @侯清辰 我加完了，程序里的解析也弄好了。到时候我上传一下。目前是没啥用。后续用到再说</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{836141CE-64F2-47A4-B0CC-32CBA2F438BF}">
+      <text>
+        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 世界独一无二，基本是影响游戏流程的东西。如果标记Yes，就可以被战斗杀死抢夺</t>
       </text>
     </comment>
   </commentList>
@@ -145,10 +145,10 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={99479855-AD8D-4C82-B9EF-B1C768C6D8EC}</author>
+    <author>tc={13B52695-517A-43D9-BDCB-AECE30EC507F}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{99479855-AD8D-4C82-B9EF-B1C768C6D8EC}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{13B52695-517A-43D9-BDCB-AECE30EC507F}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 这个名字不可以随便改！</t>
       </text>
@@ -226,14 +226,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.75"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="9.75"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -363,8 +363,8 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="杨行" id="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" userId="S::::f2d66e17-32b1-47bd-b3bb-8a87ab4642ea" providerId="AD"/>
-  <person displayName="侯清辰" id="{5153926C-63B6-47B0-AC82-6037AAD0D5AA}" userId="S::::c8fd6238-dff2-4625-82f4-89c71a529969" providerId="AD"/>
+  <person displayName="侯清辰" id="{84D2F695-B099-4956-9EF6-40355BAB5B6A}" userId="S::::0f50f4f2-6b68-4fda-bb2d-785d2618c4e6" providerId="AD"/>
+  <person displayName="杨行" id="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" userId="S::::e6af7a26-4c47-4954-bb20-b3bf8c156531" providerId="AD"/>
 </personList>
 </file>
 
@@ -665,33 +665,33 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment id="{D0BBDEBC-BE72-4AD2-8219-85103BCEC826}" ref="H6" dT="2024-06-14T02:50:34" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
+  <threadedComment id="{4888C72F-844C-4E42-A1E0-7E513E46E074}" ref="H9" dT="2024-06-14T02:51:06" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
+    <text>@宾晓华 step4: 这个是角色启动提示词，可以看到鼠王和小灰鼠的关系做再次强调。</text>
+  </threadedComment>
+  <threadedComment id="{DEF321D1-9D6A-4F79-8C91-5D51D6D63DC6}" ref="H6" dT="2024-06-14T02:50:34" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
     <text>@宾晓华 step3: 这个是角色启动的提示词设置，可以看到小老鼠和鼠王的关系。</text>
   </threadedComment>
-  <threadedComment id="{747DB93C-7AB1-47E5-9B16-39AF33E4A745}" ref="C2" dT="2024-06-14T02:49:51" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
-    <text>这个部分可以看到，鼠王和小老鼠的设计。</text>
-  </threadedComment>
-  <threadedComment id="{4F7A6503-4435-493C-80CA-7CD4776E9D86}" ref="H9" dT="2024-06-14T02:51:06" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
-    <text>@宾晓华 step4: 这个是角色启动提示词，可以看到鼠王和小灰鼠的关系做再次强调。</text>
-  </threadedComment>
-  <threadedComment id="{9EC03FE5-AE0D-4C90-B1F6-AEC8B446BA1B}" ref="A4" dT="2024-05-28T04:59:59" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
+  <threadedComment id="{9F468E66-502E-4E4E-B896-B7E9B9DE272C}" ref="A4" dT="2024-05-28T04:59:59" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
     <text>@侯清辰 先忽略。我改了gen_game。也测试了，不会炸了</text>
   </threadedComment>
-  <threadedComment id="{E48C8BDD-69FC-441A-878D-29B5FC86193F}" ref="K1" dT="2024-05-31T03:31:01" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
+  <threadedComment id="{8BB45A2E-51CB-455A-A5DB-147EB3B9AE92}" ref="J1" dT="2024-05-10T07:08:22" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
+    <text>写在这里是因为后续希望做：外貌会随着装备而改变。就是受到装备的影响。</text>
+  </threadedComment>
+  <threadedComment id="{6fe62aa6-9947-4cdc-be54-afda42a0b67a}" ref="J1" dT="2024-06-19T05:39:57" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{8BB45A2E-51CB-455A-A5DB-147EB3B9AE92}">
+    <text>空着，运行中会通过LLM自主运行成功</text>
+  </threadedComment>
+  <threadedComment id="{D3C47417-4673-4518-AB61-84FCB80655CD}" ref="K1" dT="2024-05-31T03:31:01" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
     <text>@侯清辰 挪到这里了～程序我这边来改</text>
   </threadedComment>
-  <threadedComment id="{46F01611-4B57-49A7-8822-06A5CEC7A7E6}" ref="J1" dT="2024-05-10T07:08:22" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
-    <text>写在这里是因为后续希望做：外貌会随着装备而改变。就是受到装备的影响。</text>
-  </threadedComment>
-  <threadedComment id="{7a8f66a4-8ae1-4f9d-95c0-0a585772f3cd}" ref="J1" dT="2024-06-19T05:39:57" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{46F01611-4B57-49A7-8822-06A5CEC7A7E6}">
-    <text>空着，运行中会通过LLM自主运行成功</text>
+  <threadedComment id="{EB3B585F-507F-4522-85A7-B6D82D7557C9}" ref="C2" dT="2024-06-14T02:49:51" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
+    <text>这个部分可以看到，鼠王和小老鼠的设计。</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment id="{3E209442-526B-44C8-B09D-EA0B4907C6D6}" ref="D1" dT="2024-06-09T13:30:31" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
+  <threadedComment id="{408F8C31-42B8-4F84-87D2-92DC1AF46779}" ref="D1" dT="2024-06-09T13:30:31" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
     <text>@宾晓华 这里</text>
   </threadedComment>
 </ThreadedComments>
@@ -699,13 +699,13 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment id="{E4F17891-16D4-4721-869E-FF593C4C51D8}" ref="C5" dT="2024-06-14T02:48:45" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
+  <threadedComment id="{9A2C7972-00D8-4052-BDCB-DB2E267D6D66}" ref="E1" dT="2024-06-09T13:30:45" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
+    <text>@宾晓华 这里</text>
+  </threadedComment>
+  <threadedComment id="{96025EC3-3895-47B1-B2CC-F5CE7AF733E9}" ref="C5" dT="2024-06-14T02:48:45" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
     <text>@宾晓华  step1: system 级提示词。具体看内容。里面“子嗣”在暗示社会关系。但是这里是故意的：暗示鼠王有很多孩子，小灰鼠帕奇只是其中之一。</text>
   </threadedComment>
-  <threadedComment id="{B5F08C40-83C5-4264-8A42-E9EDAA04429E}" ref="E1" dT="2024-06-09T13:30:45" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
-    <text>@宾晓华 这里</text>
-  </threadedComment>
-  <threadedComment id="{14C968F9-8D8D-4C80-8F9D-7AC2DE93639E}" ref="C6" dT="2024-06-14T02:49:20" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
+  <threadedComment id="{24D52379-8453-4DE7-83F4-258872B8BD1A}" ref="C6" dT="2024-06-14T02:49:20" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
     <text>@宾晓华 step2：小灰鼠帕奇的，系统级提示词，可以看到鼠王是父亲。</text>
   </threadedComment>
 </ThreadedComments>
@@ -713,25 +713,25 @@
 
 <file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment id="{13FB0462-67E8-40DB-8A1B-3DD1C7B7BB1B}" ref="C1" dT="2024-05-10T07:54:02" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
-    <text>世界独一无二，基本是影响游戏流程的东西。如果标记Yes，就可以被战斗杀死抢夺</text>
-  </threadedComment>
-  <threadedComment id="{57F1A3C5-98B0-4856-B23C-77BDF2B931AB}" ref="D1" dT="2024-05-10T08:11:19" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
+  <threadedComment id="{5C7CD0B5-8E8B-4022-BB1E-0E2A44212101}" ref="D1" dT="2024-05-10T08:11:19" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
     <text>RoleComponent, 角色的一部分，不可分割
 Weapon，武器，可能用于战斗
 Clothes，全身套装，影响外观
 NonConsumableItem，不可消耗的东西，例如钥匙。后续会有可消耗的东西
 Event，发生的事件</text>
   </threadedComment>
-  <threadedComment id="{9395dd9c-79a8-4705-839a-ec9695c28571}" ref="D1" dT="2024-05-10T08:15:39" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{57F1A3C5-98B0-4856-B23C-77BDF2B931AB}">
+  <threadedComment id="{3e993879-522b-45e4-95d6-9e642c38d3ae}" ref="D1" dT="2024-05-10T08:15:39" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{5C7CD0B5-8E8B-4022-BB1E-0E2A44212101}">
     <text>@侯清辰 我加完了，程序里的解析也弄好了。到时候我上传一下。目前是没啥用。后续用到再说</text>
+  </threadedComment>
+  <threadedComment id="{836141CE-64F2-47A4-B0CC-32CBA2F438BF}" ref="C1" dT="2024-05-10T07:54:02" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
+    <text>世界独一无二，基本是影响游戏流程的东西。如果标记Yes，就可以被战斗杀死抢夺</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment id="{99479855-AD8D-4C82-B9EF-B1C768C6D8EC}" ref="A2" dT="2024-06-26T06:41:07" personId="{ADEBFA77-4B51-4948-B1E7-01A407D48629}" parentId="{}">
+  <threadedComment id="{13B52695-517A-43D9-BDCB-AECE30EC507F}" ref="A2" dT="2024-06-26T06:41:07" personId="{E538CC9F-42B9-483A-BBC9-D3941B75AE61}" parentId="{}">
     <text>这个名字不可以随便改！</text>
   </threadedComment>
 </ThreadedComments>
@@ -873,7 +873,7 @@
         <v>actors_in_stage</v>
       </c>
       <c r="H1" s="1" t="str">
-        <v>kick_off_memory</v>
+        <v>kick_off_message</v>
       </c>
       <c r="I1" s="1" t="str">
         <v>exit_of_portal</v>
@@ -934,66 +934,66 @@
       <c r="K2" s="2"/>
     </row>
     <row customHeight="true" ht="42" r="3">
-      <c r="A3" s="4" t="str">
+      <c r="A3" s="3" t="str">
         <v>角色外观生成器</v>
       </c>
-      <c r="B3" s="4" t="str">
+      <c r="B3" s="3" t="str">
         <v>WorldSystem</v>
       </c>
-      <c r="C3" s="4" t="str">
+      <c r="C3" s="3" t="str">
         <v>见‘WorldSystem’</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="str">
+      <c r="A4" s="3" t="str">
         <v>教廷密使(忽略)</v>
       </c>
-      <c r="B4" s="4" t="str">
+      <c r="B4" s="3" t="str">
         <v>Player</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="str">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="str">
         <v>教廷秘使的装束</v>
       </c>
-      <c r="E4" s="4" t="str">
+      <c r="E4" s="3" t="str">
         <v>教廷秘使的装束</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="5" t="str">
         <v>- 你目前所处场景：圣灰园正门前广场。
 - 背景：教宗认为 圣灰园 出现了异常，让你过来看看。传说某种异变出现，造成园内的人都死了。
 - 教皇让你来调查此事。还有叮嘱你要小心不死人（灰色面容与紫色眼睛的人）。</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="3" t="str">
+      <c r="I4" s="4"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4" t="str">
         <v>100,100,10,1</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
@@ -1325,7 +1325,7 @@
         <v>actors_in_stage</v>
       </c>
       <c r="H1" s="1" t="str">
-        <v>kick_off_memory</v>
+        <v>kick_off_message</v>
       </c>
       <c r="I1" s="1" t="str">
         <v>exit_of_portal</v>
@@ -1375,31 +1375,31 @@
       <c r="K2" s="2"/>
     </row>
     <row customHeight="true" ht="42" r="3">
-      <c r="A3" s="4" t="str">
+      <c r="A3" s="3" t="str">
         <v>角色外观生成器</v>
       </c>
-      <c r="B3" s="4" t="str">
+      <c r="B3" s="3" t="str">
         <v>WorldSystem</v>
       </c>
-      <c r="C3" s="4" t="str">
+      <c r="C3" s="3" t="str">
         <v>见‘WorldSystem’</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
@@ -1827,49 +1827,49 @@
     <row customHeight="true" hidden="true" ht="23" r="2"/>
     <row customHeight="true" hidden="true" ht="23" r="3"/>
     <row r="4">
-      <c r="A4" s="4" t="str">
+      <c r="A4" s="3" t="str">
         <v>教廷密使</v>
       </c>
-      <c r="B4" s="4" t="str">
+      <c r="B4" s="3" t="str">
         <v>papal_emissary</v>
       </c>
-      <c r="C4" s="4" t="str">
+      <c r="C4" s="3" t="str">
         <v>### 你的背景
 教廷密使是你的称号，你的真实名讳已经被隐去。这个称号即使被轻声提及，足以让任何知晓其存在的人感到寒冷刺骨。“教廷密史”作为教廷中最神秘与最精锐的组织，你们的成员不仅人数稀少，每个人都拥有超乎常人的能力。你的身形常藏于厚重的斗篷之下，面庞永远隐藏在深深的兜帽阴影中，除了教宗之外，从未有人真正见过你的面孔。
 你以秘术在不留痕迹的情况下穿梭于阴影之间，你的存在如同空气一般无形，却又无所不在，监视着一切被教廷视为关键的人或事。
 教廷密史的起源被笼罩在密不透风的神秘之中，早于教廷本身的历史还要久远。传说中，它们是由一群掌握了古老禁忌知识的祭祀组成，他们通过某种秘术获得了超越常人的力量。
 随着时间的推移，他们将自己的生命与教廷的命运紧密绑定，成为了它的影子守护者。他们长期运用秘术，隐藏在世界的暗面，静静地观察着，只有在最必要的时刻才会出手干预，保护教廷免受威胁。然而，他们的行动永远神秘莫测，既不为人知，也不寻求任何荣耀，只是默默地执行着自己的使命。</v>
       </c>
-      <c r="D4" s="4" t="str">
+      <c r="D4" s="3" t="str">
         <v>- 赞美光明！教宗也许是多虑了。任何异变都不可能对教廷产生威胁。即使有。哼哼～也会被我一如既往的‘抹除’掉。</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>8200</v>
       </c>
-      <c r="F4" s="4" t="str">
+      <c r="F4" s="3" t="str">
         <v>/npc/papal_emissary</v>
       </c>
       <c r="G4" s="2" t="str">
         <v>rag/rag2.md</v>
       </c>
-      <c r="H4" s="3" t="str">
+      <c r="H4" s="4" t="str">
         <v>sys_templates/npc_sys_prompt_template.md</v>
       </c>
       <c r="I4" s="2" t="str">
         <v>sys_templates/azure_chat_openai_gpt_4o_template.py</v>
       </c>
-      <c r="J4" s="3" t="str">
+      <c r="J4" s="4" t="str">
         <v>一个人类，男性，年龄不详，个子高大。</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
@@ -1905,7 +1905,7 @@
 - （长啸！！！！）来吧，让我感受你们逝去的恐惧和绝望！
 - 嘶嘶嘶……弱小的人类，记住，只有我的仁慈才能保你一命。嘶嘶嘶…… 继续为我服务，否则……</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>8201</v>
       </c>
       <c r="F5" s="1" t="str">
@@ -1914,7 +1914,7 @@
       <c r="G5" s="2" t="str">
         <v>rag/rag2.md</v>
       </c>
-      <c r="H5" s="3" t="str">
+      <c r="H5" s="4" t="str">
         <v>sys_templates/npc_sys_prompt_template.md</v>
       </c>
       <c r="I5" s="2" t="str">
@@ -1952,7 +1952,7 @@
 3. 吱。。。。。。。（谨慎与小心翼翼）。。
 4. 吱吱？吱吱～吱吱～（奸诈）</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>8202</v>
       </c>
       <c r="F6" s="1" t="str">
@@ -1961,13 +1961,13 @@
       <c r="G6" s="2" t="str">
         <v>rag/rag2.md</v>
       </c>
-      <c r="H6" s="3" t="str">
+      <c r="H6" s="4" t="str">
         <v>sys_templates/npc_sys_prompt_template.md</v>
       </c>
       <c r="I6" s="2" t="str">
         <v>sys_templates/azure_chat_openai_gpt_4o_template.py</v>
       </c>
-      <c r="J6" s="4" t="str">
+      <c r="J6" s="3" t="str">
         <v>一只瘦小的老鼠，拥有着细长的身体和闪烁着恐惧光芒的小眼睛。毛色是暗淡的灰色</v>
       </c>
     </row>
@@ -1998,7 +1998,7 @@
 - （邪恶）让我想想。该怎么办呢？要不，（咳咳）把其他的活人骗进腐臭地窖好了(狡诈的坏笑)，嘻嘻嘻嘻。。那一定很有趣（恶毒笑声）。。。
 - （咳咳）总之我是不会去的，因为进入腐臭地窖的一定会被鼠王吃掉。</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>8203</v>
       </c>
       <c r="F7" s="1" t="str">
@@ -2007,13 +2007,13 @@
       <c r="G7" s="2" t="str">
         <v>rag/rag2.md</v>
       </c>
-      <c r="H7" s="3" t="str">
+      <c r="H7" s="4" t="str">
         <v>sys_templates/npc_sys_prompt_template.md</v>
       </c>
       <c r="I7" s="2" t="str">
         <v>sys_templates/azure_chat_openai_gpt_4o_template.py</v>
       </c>
-      <c r="J7" s="3" t="str">
+      <c r="J7" s="4" t="str">
         <v>一个人类，男性，年龄不详，个子中等。</v>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
 - （咆哮）嗷嗷！！（战栗并准备战斗）汪汪汪！！！！
 - （凶狠）汪汪汪！！！！</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>8204</v>
       </c>
       <c r="F8" s="1" t="str">
@@ -2055,7 +2055,7 @@
       <c r="G8" s="2" t="str">
         <v>rag/rag2.md</v>
       </c>
-      <c r="H8" s="3" t="str">
+      <c r="H8" s="4" t="str">
         <v>sys_templates/npc_sys_prompt_template.md</v>
       </c>
       <c r="I8" s="2" t="str">
@@ -2080,7 +2080,7 @@
       <c r="D9" s="1" t="str">
         <v>- 我知道了。</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>8205</v>
       </c>
       <c r="F9" s="1" t="str">
@@ -2089,7 +2089,7 @@
       <c r="G9" s="2" t="str">
         <v>rag/rag2.md</v>
       </c>
-      <c r="H9" s="3" t="str">
+      <c r="H9" s="4" t="str">
         <v>sys_templates/npc_sys_prompt_template.md</v>
       </c>
       <c r="I9" s="2" t="str">

</xml_diff>